<commit_message>
added a new line in excel
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnith\Desktop\GIT_Test\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A315CA7C-C5F0-49E9-B944-0244B37BCEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E35C42-B37F-4A18-9770-2F8CCB34BAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1428" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>test2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added this line in main branch </t>
   </si>
 </sst>
 </file>
@@ -345,9 +348,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -356,6 +361,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added a new text in excel file on the side.
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnith\Desktop\GIT_Test\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E35C42-B37F-4A18-9770-2F8CCB34BAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F70770-0B24-4C7C-930E-7588E11F6383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1428" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>test2</t>
   </si>
   <si>
     <t xml:space="preserve">added this line in main branch </t>
+  </si>
+  <si>
+    <t>added in the branch line.</t>
   </si>
 </sst>
 </file>
@@ -348,22 +351,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>